<commit_message>
Enviando a funcionalidade X
</commit_message>
<xml_diff>
--- a/GitTreino.xlsx
+++ b/GitTreino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\BetaUnityProjects\TreinoGit_N1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0EEF1A-6737-4EAC-A5C2-438D0A49921C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2388CBB9-DBBC-4CD2-89E7-4427F291BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Entrada </t>
   </si>
@@ -48,9 +48,6 @@
     <t>git add</t>
   </si>
   <si>
-    <t>Faz com que um arquivo seja enviado ao terminal e o autoriza a ser comitado.</t>
-  </si>
-  <si>
     <t>git config --global user.email "seu@email.com"</t>
   </si>
   <si>
@@ -61,6 +58,27 @@
   </si>
   <si>
     <t>Esclarece seu nome</t>
+  </si>
+  <si>
+    <t>Faz com que um arquivo seja enviado ao terminal e o autoriza a ser comitado e monitorado</t>
+  </si>
+  <si>
+    <t>Adiciona todos os arquivos da pasta e subpasta ao terminal para ser comitado</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>git commit (nome do arquivo) -m "Menssagem a ser salva"</t>
+  </si>
+  <si>
+    <t>Commita um arquivo único e atrela a uma msg.</t>
+  </si>
+  <si>
+    <t>git commit -a -m "Msg a registrar"</t>
+  </si>
+  <si>
+    <t>Commita todos os arquivos de uma vez.</t>
   </si>
 </sst>
 </file>
@@ -414,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,18 +455,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -472,7 +490,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>